<commit_message>
Added support for H2 in memory db and refactored code
</commit_message>
<xml_diff>
--- a/src/main/resources/sample_payments.xlsx
+++ b/src/main/resources/sample_payments.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ragiv/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ragiv/Desktop/payments/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>uber_user_uuid</t>
   </si>
@@ -156,13 +157,184 @@
   </si>
   <si>
     <t>pbl00019</t>
+  </si>
+  <si>
+    <t>Pandu Naik. R</t>
+  </si>
+  <si>
+    <t>TS12UB1401</t>
+  </si>
+  <si>
+    <t>abc923ef-9b54-4903-b796-fc045517b613</t>
+  </si>
+  <si>
+    <t>Venkatesh .B</t>
+  </si>
+  <si>
+    <t>7989613784, 9490317246</t>
+  </si>
+  <si>
+    <t>TS08UA7041</t>
+  </si>
+  <si>
+    <t>7f317c03-abd1-417c-b861-57ee818b1627</t>
+  </si>
+  <si>
+    <t>Kashanna .M</t>
+  </si>
+  <si>
+    <t>9010668912, 9010992356</t>
+  </si>
+  <si>
+    <t>TS32T0226</t>
+  </si>
+  <si>
+    <t>surname diffrent</t>
+  </si>
+  <si>
+    <t>7dd64b23-fd3f-47ef-9b09-f78ffdd50761</t>
+  </si>
+  <si>
+    <t>Sameer Bin Ghalib</t>
+  </si>
+  <si>
+    <t>9030575021, 7331135665</t>
+  </si>
+  <si>
+    <t>TS12UA9901</t>
+  </si>
+  <si>
+    <t>fca6618e-51ab-46f0-805d-94b63775e1c6</t>
+  </si>
+  <si>
+    <t>Emmadi Venkata Krishna</t>
+  </si>
+  <si>
+    <t>8978590941, 9908163641</t>
+  </si>
+  <si>
+    <t>TS10Y3797- TR</t>
+  </si>
+  <si>
+    <t>4fc955a8-c217-45be-b202-c7f27d653632</t>
+  </si>
+  <si>
+    <t>S. Eswar</t>
+  </si>
+  <si>
+    <t>9542237202, 9502133206</t>
+  </si>
+  <si>
+    <t>AP09TVA2420</t>
+  </si>
+  <si>
+    <t>ab38477d-061f-4447-80d5-3fc36aa9860d</t>
+  </si>
+  <si>
+    <t>Srinivas Reddy Kodala</t>
+  </si>
+  <si>
+    <t>9100098028, 7989279370</t>
+  </si>
+  <si>
+    <t>TS07UB8028</t>
+  </si>
+  <si>
+    <t>dfc999b9-f6a9-457f-84d8-f7d268ff55f2</t>
+  </si>
+  <si>
+    <t>Mohammed Sameer</t>
+  </si>
+  <si>
+    <t>9100168748, 8801238226</t>
+  </si>
+  <si>
+    <t>TS13UA6307</t>
+  </si>
+  <si>
+    <t>01e40913-caed-4a64-aad0-e9df8e0f5b37</t>
+  </si>
+  <si>
+    <t>Kiran Kumar .P</t>
+  </si>
+  <si>
+    <t>8184882303, 9010189800</t>
+  </si>
+  <si>
+    <t>Ap28VA1134</t>
+  </si>
+  <si>
+    <t>69240fd8-af19-4d0a-b600-b1c8cd719167</t>
+  </si>
+  <si>
+    <t>Lavudya Ganesh</t>
+  </si>
+  <si>
+    <t>9949492597, 7893506681</t>
+  </si>
+  <si>
+    <t>TS12UA9809</t>
+  </si>
+  <si>
+    <t>45afdd58-fd5d-435a-8809-7e1cb6eca87d</t>
+  </si>
+  <si>
+    <t>J. Vijaya Reddy</t>
+  </si>
+  <si>
+    <t>9666938887, 9347283677</t>
+  </si>
+  <si>
+    <t>TS08UB6613</t>
+  </si>
+  <si>
+    <t>c19be4da-2a19-4710-9507-1b5d479cf110</t>
+  </si>
+  <si>
+    <t>Srinivasulu Reddy. L</t>
+  </si>
+  <si>
+    <t>9700335473, 8374948834</t>
+  </si>
+  <si>
+    <t>TS15UA7264</t>
+  </si>
+  <si>
+    <t>84d609db-6821-4ac0-b51f-ce84dc52cab4</t>
+  </si>
+  <si>
+    <t>V.Srinivas Rao</t>
+  </si>
+  <si>
+    <t>9550325414, 9951303065</t>
+  </si>
+  <si>
+    <t>TS07AB6412- TR</t>
+  </si>
+  <si>
+    <t>payment issue</t>
+  </si>
+  <si>
+    <t>54e578ae-1829-4392-afc1-1c8f9ff4e2e9</t>
+  </si>
+  <si>
+    <t>Srinivasulu .P</t>
+  </si>
+  <si>
+    <t>9640121375, 9441643556</t>
+  </si>
+  <si>
+    <t>AP09TVA2726</t>
+  </si>
+  <si>
+    <t>ebd08a25-a92c-4691-b72a-f3f9933e982c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +347,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -198,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -206,6 +390,9 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,4 +1021,277 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3">
+        <v>9948207791</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed implementation to not include uber id while creating partner. Added support to export partners with out uber id.
</commit_message>
<xml_diff>
--- a/src/main/resources/sample_payments.xlsx
+++ b/src/main/resources/sample_payments.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -343,13 +344,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -359,6 +353,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -384,15 +385,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,348 +674,353 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>2200</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>2200</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>2200</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>2200</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1930</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>1930</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>1860</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>662</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>1198</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>1860</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>1860</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>1800</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>1800</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>1960</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>1960</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>2240</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>3.11</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>2236.89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>2300</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>966.08</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>1333.92</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>1780</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>1780</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>2230</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>2230</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>2132</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>272.18</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>1859.82</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>1656</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>1656</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>2480</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>2480</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>2206</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>2206</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>2206</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>233.27</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>1972.73</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>2082</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>27.95</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>2054.0500000000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <v>2168</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>2168</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>1988</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>1988</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1028,270 +1034,287 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="1">
         <v>9948207791</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>